<commit_message>
update vacc data for corona report
</commit_message>
<xml_diff>
--- a/data/kbvreport_export/faktenblatttabellen_2021-05-09.xlsx
+++ b/data/kbvreport_export/faktenblatttabellen_2021-05-09.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="346">
   <si>
     <t xml:space="preserve">Testungen</t>
   </si>
@@ -777,7 +777,7 @@
     <t xml:space="preserve">Geimpfte Personen</t>
   </si>
   <si>
-    <t xml:space="preserve">Stand 11.5.</t>
+    <t xml:space="preserve">Stand 12.5.</t>
   </si>
   <si>
     <t xml:space="preserve">Anteil_Veraenderung</t>
@@ -786,22 +786,22 @@
     <t xml:space="preserve"/>
   </si>
   <si>
-    <t xml:space="preserve">23860165 (28,7 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27711114 (33,3 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4,6 PP</t>
+    <t xml:space="preserve">24546919 (29,5 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28544440 (34,3 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4,8 PP</t>
   </si>
   <si>
     <t xml:space="preserve">Nicht vollst. geimpft</t>
   </si>
   <si>
-    <t xml:space="preserve">17088689 (20,5 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19688224 (23,7 %)</t>
+    <t xml:space="preserve">17615335 (21,2 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20223760 (24,3 %)</t>
   </si>
   <si>
     <t xml:space="preserve">3,1 PP</t>
@@ -810,13 +810,13 @@
     <t xml:space="preserve">Vollst. geimpft</t>
   </si>
   <si>
-    <t xml:space="preserve">6771476 ( 8,1 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8022890 ( 9,6 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,5 PP</t>
+    <t xml:space="preserve">6931584 ( 8,3 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8320680 (10,0 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,7 PP</t>
   </si>
   <si>
     <t xml:space="preserve">Impffortschritt</t>
@@ -870,85 +870,100 @@
     <t xml:space="preserve">Gesamt vollst.</t>
   </si>
   <si>
-    <t xml:space="preserve">33,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 9,6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">32,6</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 9,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33,9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 9,9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">34,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 8,9</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 8,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">35,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">34,6</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 8,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">35,3</t>
+    <t xml:space="preserve">34,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">35,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">36,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">35,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">36,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">38,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33,6</t>
   </si>
   <si>
     <t xml:space="preserve">31,9</t>
   </si>
   <si>
-    <t xml:space="preserve">37,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">32,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 9,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">31,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13,9</t>
+    <t xml:space="preserve">11,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14,4</t>
   </si>
   <si>
     <t xml:space="preserve">Impfstoffdosen</t>
@@ -960,28 +975,28 @@
     <t xml:space="preserve">Biontech/Pfizer</t>
   </si>
   <si>
-    <t xml:space="preserve">22768239 (74,3 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26318180 (73,7 %)</t>
+    <t xml:space="preserve">23399097 (74,4 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27168667 (73,8 %)</t>
   </si>
   <si>
     <t xml:space="preserve">Erstimpfungen</t>
   </si>
   <si>
-    <t xml:space="preserve">16515448</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19088134</t>
+    <t xml:space="preserve">17014901</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19701594</t>
   </si>
   <si>
     <t xml:space="preserve">Zweitimpfungen</t>
   </si>
   <si>
-    <t xml:space="preserve">6252791</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7230046</t>
+    <t xml:space="preserve">6384196</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7467073</t>
   </si>
   <si>
     <t xml:space="preserve">geliefert</t>
@@ -996,22 +1011,22 @@
     <t xml:space="preserve">Moderna</t>
   </si>
   <si>
-    <t xml:space="preserve">1872526 ( 6,1 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2375361 ( 6,7 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1435533</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1809562</t>
-  </si>
-  <si>
-    <t xml:space="preserve">436993</t>
-  </si>
-  <si>
-    <t xml:space="preserve">565799</t>
+    <t xml:space="preserve">1932692 ( 6,1 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2463861 ( 6,7 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1482621</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1870450</t>
+  </si>
+  <si>
+    <t xml:space="preserve">450071</t>
+  </si>
+  <si>
+    <t xml:space="preserve">593411</t>
   </si>
   <si>
     <t xml:space="preserve">3118800</t>
@@ -1023,22 +1038,22 @@
     <t xml:space="preserve">AstraZeneca</t>
   </si>
   <si>
-    <t xml:space="preserve">5975398 (19,5 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6991965 (19,6 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5901445</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6789169</t>
-  </si>
-  <si>
-    <t xml:space="preserve">73953</t>
-  </si>
-  <si>
-    <t xml:space="preserve">202796</t>
+    <t xml:space="preserve">6127132 (19,5 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7176720 (19,5 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6039606</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6944460</t>
+  </si>
+  <si>
+    <t xml:space="preserve">87526</t>
+  </si>
+  <si>
+    <t xml:space="preserve">232260</t>
   </si>
   <si>
     <t xml:space="preserve">8450400</t>
@@ -1047,10 +1062,10 @@
     <t xml:space="preserve">Johnson&amp;Johnson</t>
   </si>
   <si>
-    <t xml:space="preserve">7739 ( 0,0 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24249 ( 0,1 %)</t>
+    <t xml:space="preserve">9791 ( 0,0 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27936 ( 0,1 %)</t>
   </si>
   <si>
     <t xml:space="preserve">473400</t>
@@ -1638,7 +1653,7 @@
         <v>283</v>
       </c>
       <c r="D4" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="E4" t="n">
         <v>106</v>
@@ -1655,10 +1670,10 @@
         <v>91933</v>
       </c>
       <c r="C5" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D5" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="E5" t="n">
         <v>87</v>
@@ -1675,10 +1690,10 @@
         <v>77876</v>
       </c>
       <c r="C6" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E6" t="n">
         <v>81</v>
@@ -1695,10 +1710,10 @@
         <v>16164</v>
       </c>
       <c r="C7" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D7" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="E7" t="n">
         <v>90</v>
@@ -1715,10 +1730,10 @@
         <v>41480</v>
       </c>
       <c r="C8" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D8" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="E8" t="n">
         <v>67</v>
@@ -1735,10 +1750,10 @@
         <v>155826</v>
       </c>
       <c r="C9" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="D9" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="E9" t="n">
         <v>117</v>
@@ -1755,10 +1770,10 @@
         <v>60758</v>
       </c>
       <c r="C10" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="D10" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="E10" t="n">
         <v>78</v>
@@ -1775,10 +1790,10 @@
         <v>211481</v>
       </c>
       <c r="C11" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="D11" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="E11" t="n">
         <v>78</v>
@@ -1795,7 +1810,7 @@
         <v>510837</v>
       </c>
       <c r="C12" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="D12" t="s">
         <v>292</v>
@@ -1815,10 +1830,10 @@
         <v>102537</v>
       </c>
       <c r="C13" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="D13" t="s">
-        <v>285</v>
+        <v>301</v>
       </c>
       <c r="E13" t="n">
         <v>93</v>
@@ -1835,10 +1850,10 @@
         <v>28266</v>
       </c>
       <c r="C14" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="D14" t="s">
-        <v>287</v>
+        <v>303</v>
       </c>
       <c r="E14" t="n">
         <v>102</v>
@@ -1855,10 +1870,10 @@
         <v>96387</v>
       </c>
       <c r="C15" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="D15" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="E15" t="n">
         <v>145</v>
@@ -1875,10 +1890,10 @@
         <v>56623</v>
       </c>
       <c r="C16" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="D16" t="s">
-        <v>302</v>
+        <v>280</v>
       </c>
       <c r="E16" t="n">
         <v>115</v>
@@ -1895,10 +1910,10 @@
         <v>77368</v>
       </c>
       <c r="C17" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="D17" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="E17" t="n">
         <v>49</v>
@@ -1915,10 +1930,10 @@
         <v>52713</v>
       </c>
       <c r="C18" t="s">
-        <v>284</v>
+        <v>309</v>
       </c>
       <c r="D18" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="E18" t="n">
         <v>168</v>
@@ -1943,167 +1958,167 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="B2" t="s">
-        <v>309</v>
+        <v>314</v>
       </c>
       <c r="C2" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="B3" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="C3" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="B4" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="C4" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="B5" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="C5" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="B6" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
       <c r="C6" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="B7" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="C7" t="s">
-        <v>324</v>
+        <v>329</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="B8" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="C8" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="B9" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="C9" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
       <c r="B10" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="C10" t="s">
-        <v>331</v>
+        <v>336</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="B11" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="C11" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="B12" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
       <c r="C12" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="B13" t="s">
-        <v>336</v>
+        <v>341</v>
       </c>
       <c r="C13" t="s">
-        <v>336</v>
+        <v>341</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>337</v>
+        <v>342</v>
       </c>
       <c r="B14" t="s">
-        <v>338</v>
+        <v>343</v>
       </c>
       <c r="C14" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="B15" t="s">
-        <v>340</v>
+        <v>345</v>
       </c>
       <c r="C15" t="s">
-        <v>340</v>
+        <v>345</v>
       </c>
     </row>
   </sheetData>

</xml_diff>